<commit_message>
bug fixes and updates
</commit_message>
<xml_diff>
--- a/kobetran_resources.xlsx
+++ b/kobetran_resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kobetran/Documents/Personal_Projects/WebDevelopment/kobetran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFEB7E0-0AF4-104A-8109-758BA70DC461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D33872-2154-BD42-BB77-85FA5EC7F106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16120" yWindow="5960" windowWidth="28100" windowHeight="17440" xr2:uid="{155398B1-E7AE-E84A-818D-5D1E3818DDD4}"/>
+    <workbookView xWindow="20100" yWindow="7100" windowWidth="28100" windowHeight="17440" xr2:uid="{155398B1-E7AE-E84A-818D-5D1E3818DDD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>